<commit_message>
pgmm daily and weekly inputs
</commit_message>
<xml_diff>
--- a/data/raw/regions/CentralAsia-Results.xlsx
+++ b/data/raw/regions/CentralAsia-Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Dropbox (Personal)\COVID Survellance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Global-COVID-Surveillance\data\raw\regions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{595805C0-601D-4552-B842-E186D722AD20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E56DC1-C709-4615-913C-2732F2B9E02F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27165" yWindow="2475" windowWidth="21765" windowHeight="14895"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CentralAsia-Results" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -584,11 +584,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -943,25 +947,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="10.15625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.41796875" customWidth="1"/>
+    <col min="8" max="8" width="12.41796875" customWidth="1"/>
+    <col min="12" max="12" width="12.578125" customWidth="1"/>
+    <col min="14" max="14" width="11.26171875" customWidth="1"/>
     <col min="15" max="16" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1007,8 +1010,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3">
         <v>44110</v>
       </c>
       <c r="B2" t="s">
@@ -1054,8 +1057,8 @@
         <v>-0.55477630072740702</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3">
         <v>44117</v>
       </c>
       <c r="B3" t="s">
@@ -1101,8 +1104,8 @@
         <v>-0.79019614544073902</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3">
         <v>44110</v>
       </c>
       <c r="B4" t="s">
@@ -1148,8 +1151,8 @@
         <v>-5.4300034275892001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3">
         <v>44117</v>
       </c>
       <c r="B5" t="s">
@@ -1195,8 +1198,8 @@
         <v>-5.9502871568183902E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3">
         <v>44110</v>
       </c>
       <c r="B6" t="s">
@@ -1242,8 +1245,8 @@
         <v>-7.6601663834519898E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3">
         <v>44117</v>
       </c>
       <c r="B7" t="s">
@@ -1289,8 +1292,8 @@
         <v>-8.1504170319929195E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3">
         <v>44110</v>
       </c>
       <c r="B8" t="s">
@@ -1336,8 +1339,8 @@
         <v>-0.38557433084470899</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3">
         <v>44117</v>
       </c>
       <c r="B9" t="s">
@@ -1383,8 +1386,8 @@
         <v>-0.66710479463608496</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3">
         <v>44110</v>
       </c>
       <c r="B10" t="s">
@@ -1430,8 +1433,8 @@
         <v>-1.81702233367202E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3">
         <v>44117</v>
       </c>
       <c r="B11" t="s">
@@ -1477,8 +1480,8 @@
         <v>-1.8011531429849299E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3">
         <v>44110</v>
       </c>
       <c r="B12" t="s">
@@ -1524,8 +1527,8 @@
         <v>-0.149827667784379</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3">
         <v>44117</v>
       </c>
       <c r="B13" t="s">
@@ -1571,8 +1574,8 @@
         <v>-0.128950041945572</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="3">
         <v>44110</v>
       </c>
       <c r="B14" t="s">
@@ -1618,8 +1621,8 @@
         <v>-0.111479604696806</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="3">
         <v>44117</v>
       </c>
       <c r="B15" t="s">
@@ -1665,8 +1668,8 @@
         <v>-0.145264750201858</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="3">
         <v>44110</v>
       </c>
       <c r="B16" t="s">
@@ -1712,8 +1715,8 @@
         <v>-0.32398429439808502</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="3">
         <v>44117</v>
       </c>
       <c r="B17" t="s">
@@ -1759,8 +1762,8 @@
         <v>-0.46182744903317902</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3">
         <v>44110</v>
       </c>
       <c r="B18" t="s">
@@ -1806,8 +1809,8 @@
         <v>-0.26084204865856597</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="3">
         <v>44117</v>
       </c>
       <c r="B19" t="s">
@@ -1853,8 +1856,8 @@
         <v>-0.350270410331252</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="3">
         <v>44110</v>
       </c>
       <c r="B20" t="s">
@@ -1900,8 +1903,8 @@
         <v>-2.31674048768108E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="3">
         <v>44117</v>
       </c>
       <c r="B21" t="s">
@@ -1947,8 +1950,8 @@
         <v>-2.26946006956514E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="3">
         <v>44110</v>
       </c>
       <c r="B22" t="s">
@@ -1994,8 +1997,8 @@
         <v>-9.6578352553408506E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="3">
         <v>44117</v>
       </c>
       <c r="B23" t="s">
@@ -2041,8 +2044,8 @@
         <v>-9.0547707931796395E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3">
         <v>44110</v>
       </c>
       <c r="B24" t="s">
@@ -2088,8 +2091,8 @@
         <v>-8.0251289272019799E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="3">
         <v>44117</v>
       </c>
       <c r="B25" t="s">
@@ -2135,8 +2138,8 @@
         <v>-6.5377787853384398E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="3">
         <v>44110</v>
       </c>
       <c r="B26" t="s">
@@ -2182,8 +2185,8 @@
         <v>-0.16214282140853101</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="3">
         <v>44117</v>
       </c>
       <c r="B27" t="s">

</xml_diff>